<commit_message>
Clean up + new report data
</commit_message>
<xml_diff>
--- a/a3/reportData.xlsx
+++ b/a3/reportData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nolan\Documents\_School\_f19\languageProcessing\a3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nolan\Documents\school\languageProcessing\a3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6A18536-05F8-4E2B-80A4-845915564A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D397FFE-6A26-4BE0-BB95-6822364E4E8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{0D1C9DCD-F322-43BD-9C40-508B856E9105}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0D1C9DCD-F322-43BD-9C40-508B856E9105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SelectKBest + Knearest</t>
   </si>
@@ -56,12 +55,6 @@
   </si>
   <si>
     <t>SelectFpr + MLP</t>
-  </si>
-  <si>
-    <t>Improving the preprocessing</t>
-  </si>
-  <si>
-    <t>need to redo left with new alpha vals</t>
   </si>
 </sst>
 </file>
@@ -255,22 +248,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.63333333333333297</c:v>
+                  <c:v>0.62752446150516505</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64</c:v>
+                  <c:v>0.55776075935713498</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.61</c:v>
+                  <c:v>0.56043956043956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64</c:v>
+                  <c:v>0.53729041245833098</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62</c:v>
+                  <c:v>0.55601544921851498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60666666666666602</c:v>
+                  <c:v>0.52447283731206995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -345,24 +338,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.64666666666666595</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.62333333333333296</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.63333333333333297</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.63333333333333297</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62333333333333296</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.64333333333333298</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -450,7 +425,8 @@
         <c:axId val="385311824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -517,37 +493,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -731,22 +676,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.63</c:v>
+                  <c:v>0.567702579374609</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62333333333333296</c:v>
+                  <c:v>0.54641000110631699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.63333333333333297</c:v>
+                  <c:v>0.54045905465862598</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63</c:v>
+                  <c:v>0.55394844833533496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62666666666666604</c:v>
+                  <c:v>0.53882962123926503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64666666666666595</c:v>
+                  <c:v>0.55429685686429198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,24 +766,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.62333333333333296</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.63666666666666605</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.61666666666666603</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.63666666666666605</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.67333333333333301</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -929,8 +856,8 @@
         <c:axId val="382485712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
-          <c:min val="0.60000000000000009"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -997,37 +924,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1211,22 +1107,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.82666666666666599</c:v>
+                  <c:v>0.76956729859402595</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82666666666666599</c:v>
+                  <c:v>0.79329658605974396</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82</c:v>
+                  <c:v>0.82663584637268805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83333333333333304</c:v>
+                  <c:v>0.83999288857282495</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.836666666666666</c:v>
+                  <c:v>0.83662128368991295</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84666666666666601</c:v>
+                  <c:v>0.83997155049786598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,24 +1197,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.83333333333333304</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.836666666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.85333333333333306</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.85</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1406,8 +1284,8 @@
         <c:axId val="315030256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.9"/>
-          <c:min val="0.8"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1474,37 +1352,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1688,22 +1535,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.82</c:v>
+                  <c:v>0.77996088193456603</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83</c:v>
+                  <c:v>0.823315664899823</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82666666666666599</c:v>
+                  <c:v>0.80665807369216402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84</c:v>
+                  <c:v>0.84331766509984296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83</c:v>
+                  <c:v>0.83332592559669305</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.836666666666666</c:v>
+                  <c:v>0.84333159257324997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1778,24 +1625,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.836666666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.85666666666666602</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.85666666666666602</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1888,8 +1717,8 @@
         <c:axId val="623625688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.9"/>
-          <c:min val="0.8"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1947,6 +1776,7 @@
         <c:crossAx val="623625360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1956,37 +1786,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2170,22 +1969,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.83</c:v>
+                  <c:v>0.81632175974886101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86333333333333295</c:v>
+                  <c:v>0.86992918366666305</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.86</c:v>
+                  <c:v>0.87997866287339899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87333333333333296</c:v>
+                  <c:v>0.85994397759103602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.87</c:v>
+                  <c:v>0.86992918366666305</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.87333333333333296</c:v>
+                  <c:v>0.876555566676675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2260,24 +2059,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.85666666666666602</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.87333333333333296</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.87333333333333296</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.88333333333333297</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2365,8 +2146,8 @@
         <c:axId val="374871840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.93"/>
-          <c:min val="0.83000000000000007"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2424,7 +2205,7 @@
         <c:crossAx val="374870856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1.0000000000000002E-2"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2434,37 +2215,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2648,22 +2398,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
+                  <c:v>0.85322896281800298</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85333333333333306</c:v>
+                  <c:v>0.88994007848717605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87666666666666604</c:v>
+                  <c:v>0.86661331199146296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85666666666666602</c:v>
+                  <c:v>0.85977564102563997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88</c:v>
+                  <c:v>0.86967418546365904</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88</c:v>
+                  <c:v>0.88326978021367097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2738,24 +2488,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.87666666666666604</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.89333333333333298</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.89666666666666595</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.92333333333333301</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2845,8 +2577,8 @@
         <c:axId val="388330768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.93"/>
-          <c:min val="0.83000000000000007"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2913,37 +2645,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -6328,16 +6029,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>59403</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3379</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1081380</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>75096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>114709</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>58071</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>679486</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129788</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6364,16 +6065,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>259120</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>868721</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>177492</xdr:rowOff>
+      <xdr:rowOff>69915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>314427</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>52950</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>422004</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>124667</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6400,16 +6101,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>100370</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23862</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1086488</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>158333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>155676</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>684594</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>78554</xdr:rowOff>
+      <xdr:rowOff>33731</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6436,16 +6137,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>335935</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>34105</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>882782</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>159611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>391242</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>436065</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>88797</xdr:rowOff>
+      <xdr:rowOff>35009</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6472,16 +6173,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>115733</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1092887</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>39226</xdr:rowOff>
+      <xdr:rowOff>48190</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171039</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>690993</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>93918</xdr:rowOff>
+      <xdr:rowOff>102882</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6508,16 +6209,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>351298</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>907111</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>75073</xdr:rowOff>
+      <xdr:rowOff>48178</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>406605</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>460394</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>129765</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6842,25 +6543,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F965E7C4-A30F-4B3C-89AE-6A97A5690BBC}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q55"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6870,894 +6571,426 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>500</v>
       </c>
       <c r="B2">
-        <v>0.58764705882352897</v>
+        <v>0.60117647058823498</v>
       </c>
       <c r="C2">
-        <v>0.63333333333333297</v>
-      </c>
-      <c r="G2">
-        <v>500</v>
-      </c>
-      <c r="H2">
-        <v>0.59058823529411697</v>
-      </c>
-      <c r="I2">
-        <v>0.64666666666666595</v>
+        <v>0.62752446150516505</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1000</v>
       </c>
       <c r="B3">
-        <v>0.59882352941176398</v>
+        <v>0.59</v>
       </c>
       <c r="C3">
-        <v>0.64</v>
-      </c>
-      <c r="G3">
-        <v>1000</v>
-      </c>
-      <c r="H3">
-        <v>0.60529411764705798</v>
-      </c>
-      <c r="I3">
-        <v>0.62333333333333296</v>
+        <v>0.55776075935713498</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1500</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.57411764705882296</v>
       </c>
       <c r="C4">
-        <v>0.61</v>
-      </c>
-      <c r="G4">
-        <v>1500</v>
-      </c>
-      <c r="H4">
-        <v>0.60411764705882298</v>
-      </c>
-      <c r="I4">
-        <v>0.63333333333333297</v>
+        <v>0.56043956043956</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2000</v>
       </c>
       <c r="B5">
-        <v>0.60294117647058798</v>
+        <v>0.57411764705882296</v>
       </c>
       <c r="C5">
-        <v>0.64</v>
-      </c>
-      <c r="G5">
-        <v>2000</v>
-      </c>
-      <c r="H5">
-        <v>0.61058823529411699</v>
-      </c>
-      <c r="I5">
-        <v>0.63333333333333297</v>
+        <v>0.53729041245833098</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2500</v>
       </c>
       <c r="B6">
-        <v>0.60588235294117598</v>
+        <v>0.58176470588235296</v>
       </c>
       <c r="C6">
-        <v>0.62</v>
-      </c>
-      <c r="G6">
-        <v>2500</v>
-      </c>
-      <c r="H6">
-        <v>0.624705882352941</v>
-      </c>
-      <c r="I6">
-        <v>0.62333333333333296</v>
+        <v>0.55601544921851498</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3000</v>
       </c>
       <c r="B7">
-        <v>0.60588235294117598</v>
+        <v>0.56823529411764695</v>
       </c>
       <c r="C7">
-        <v>0.60666666666666602</v>
-      </c>
-      <c r="G7">
-        <v>3000</v>
-      </c>
-      <c r="H7">
-        <v>0.625882352941176</v>
-      </c>
-      <c r="I7">
-        <v>0.64333333333333298</v>
+        <v>0.52447283731206995</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D8">
-        <v>0.58823529411764697</v>
-      </c>
-      <c r="E8">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>0.59058823529411697</v>
-      </c>
-      <c r="E9">
-        <v>0.64</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1E-3</v>
       </c>
       <c r="B10">
-        <v>0.59176470588235297</v>
+        <v>0.60352941176470498</v>
       </c>
       <c r="C10">
-        <v>0.63</v>
-      </c>
-      <c r="D10">
-        <v>0.59176470588235297</v>
-      </c>
-      <c r="E10">
-        <v>0.63</v>
-      </c>
-      <c r="G10">
-        <v>1E-3</v>
-      </c>
-      <c r="H10">
-        <v>0.59941176470588198</v>
-      </c>
-      <c r="I10">
-        <v>0.62333333333333296</v>
+        <v>0.567702579374609</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B11">
-        <v>0.59588235294117597</v>
+        <v>0.58411764705882296</v>
       </c>
       <c r="C11">
-        <v>0.62333333333333296</v>
-      </c>
-      <c r="D11">
-        <v>0.59588235294117597</v>
-      </c>
-      <c r="E11">
-        <v>0.62333333333333296</v>
-      </c>
-      <c r="G11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H11">
-        <v>0.6</v>
-      </c>
-      <c r="I11">
-        <v>0.63666666666666605</v>
+        <v>0.54641000110631699</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.01</v>
       </c>
       <c r="B12">
-        <v>0.60235294117646998</v>
+        <v>0.57882352941176396</v>
       </c>
       <c r="C12">
-        <v>0.63333333333333297</v>
-      </c>
-      <c r="D12">
-        <v>0.60235294117646998</v>
-      </c>
-      <c r="E12">
-        <v>0.63333333333333297</v>
-      </c>
-      <c r="G12">
-        <v>0.01</v>
-      </c>
-      <c r="H12">
-        <v>0.60352941176470498</v>
-      </c>
-      <c r="I12">
-        <v>0.61666666666666603</v>
+        <v>0.54045905465862598</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.05</v>
       </c>
       <c r="B13">
-        <v>0.59058823529411697</v>
+        <v>0.55882352941176405</v>
       </c>
       <c r="C13">
-        <v>0.63</v>
-      </c>
-      <c r="D13">
-        <v>0.59058823529411697</v>
-      </c>
-      <c r="E13">
-        <v>0.63</v>
-      </c>
-      <c r="G13">
-        <v>0.05</v>
-      </c>
-      <c r="H13">
-        <v>0.61470588235294099</v>
-      </c>
-      <c r="I13">
-        <v>0.63666666666666605</v>
+        <v>0.55394844833533496</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.1</v>
       </c>
       <c r="B14">
-        <v>0.59</v>
+        <v>0.56411764705882295</v>
       </c>
       <c r="C14">
-        <v>0.62666666666666604</v>
-      </c>
-      <c r="G14">
-        <v>0.1</v>
-      </c>
-      <c r="H14">
-        <v>0.61764705882352899</v>
-      </c>
-      <c r="I14">
-        <v>0.65</v>
+        <v>0.53882962123926503</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.5</v>
       </c>
       <c r="B15">
-        <v>0.61647058823529399</v>
+        <v>0.56352941176470595</v>
       </c>
       <c r="C15">
-        <v>0.64666666666666595</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <v>0.63235294117647001</v>
-      </c>
-      <c r="I15">
-        <v>0.67333333333333301</v>
+        <v>0.55429685686429198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>500</v>
       </c>
       <c r="B19">
-        <v>0.80647058823529405</v>
+        <v>0.8</v>
       </c>
       <c r="C19">
-        <v>0.82666666666666599</v>
-      </c>
-      <c r="G19">
-        <v>500</v>
-      </c>
-      <c r="H19">
-        <v>0.81294117647058795</v>
-      </c>
-      <c r="I19">
-        <v>0.83333333333333304</v>
+        <v>0.76956729859402595</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1000</v>
       </c>
       <c r="B20">
-        <v>0.81235294117646994</v>
+        <v>0.80882352941176405</v>
       </c>
       <c r="C20">
-        <v>0.82666666666666599</v>
-      </c>
-      <c r="G20">
-        <v>1000</v>
-      </c>
-      <c r="H20">
-        <v>0.82647058823529396</v>
-      </c>
-      <c r="I20">
-        <v>0.836666666666666</v>
+        <v>0.79329658605974396</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1500</v>
       </c>
       <c r="B21">
-        <v>0.81588235294117595</v>
+        <v>0.80882352941176405</v>
       </c>
       <c r="C21">
-        <v>0.82</v>
-      </c>
-      <c r="G21">
-        <v>1500</v>
-      </c>
-      <c r="H21">
-        <v>0.82764705882352896</v>
-      </c>
-      <c r="I21">
-        <v>0.86</v>
+        <v>0.82663584637268805</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2000</v>
       </c>
       <c r="B22">
-        <v>0.81411764705882295</v>
+        <v>0.80764705882352905</v>
       </c>
       <c r="C22">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="G22">
-        <v>2000</v>
-      </c>
-      <c r="H22">
-        <v>0.83176470588235296</v>
-      </c>
-      <c r="I22">
-        <v>0.85</v>
+        <v>0.83999288857282495</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2500</v>
       </c>
       <c r="B23">
-        <v>0.81529411764705795</v>
+        <v>0.81352941176470595</v>
       </c>
       <c r="C23">
-        <v>0.836666666666666</v>
-      </c>
-      <c r="G23">
-        <v>2500</v>
-      </c>
-      <c r="H23">
-        <v>0.83</v>
-      </c>
-      <c r="I23">
-        <v>0.85333333333333306</v>
+        <v>0.83662128368991295</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3000</v>
       </c>
       <c r="B24">
-        <v>0.81529411764705795</v>
+        <v>0.81411764705882295</v>
       </c>
       <c r="C24">
-        <v>0.84666666666666601</v>
-      </c>
-      <c r="G24">
-        <v>3000</v>
-      </c>
-      <c r="H24">
-        <v>0.82705882352941096</v>
-      </c>
-      <c r="I24">
-        <v>0.85</v>
+        <v>0.83997155049786598</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D25">
-        <v>0.79647058823529404</v>
-      </c>
-      <c r="E25">
-        <v>0.82333333333333303</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
-        <v>0.80235294117647005</v>
-      </c>
-      <c r="E26">
-        <v>0.80666666666666598</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1E-3</v>
       </c>
       <c r="B27">
-        <v>0.81352941176470495</v>
+        <v>0.79470588235294104</v>
       </c>
       <c r="C27">
-        <v>0.82</v>
-      </c>
-      <c r="D27">
-        <v>0.81352941176470495</v>
-      </c>
-      <c r="E27">
-        <v>0.82</v>
-      </c>
-      <c r="G27">
-        <v>1E-3</v>
-      </c>
-      <c r="H27">
-        <v>0.81529411764705795</v>
-      </c>
-      <c r="I27">
-        <v>0.836666666666666</v>
+        <v>0.77996088193456603</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B28">
-        <v>0.81529411764705795</v>
+        <v>0.81058823529411705</v>
       </c>
       <c r="C28">
-        <v>0.83</v>
-      </c>
-      <c r="D28">
-        <v>0.81529411764705795</v>
-      </c>
-      <c r="E28">
-        <v>0.83</v>
-      </c>
-      <c r="G28">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H28">
-        <v>0.82882352941176396</v>
-      </c>
-      <c r="I28">
-        <v>0.86</v>
+        <v>0.823315664899823</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.01</v>
       </c>
       <c r="B29">
-        <v>0.81470588235294095</v>
+        <v>0.80941176470588205</v>
       </c>
       <c r="C29">
-        <v>0.82666666666666599</v>
-      </c>
-      <c r="D29">
-        <v>0.81470588235294095</v>
-      </c>
-      <c r="E29">
-        <v>0.82666666666666599</v>
-      </c>
-      <c r="G29">
-        <v>0.01</v>
-      </c>
-      <c r="H29">
-        <v>0.83058823529411696</v>
-      </c>
-      <c r="I29">
-        <v>0.85</v>
+        <v>0.80665807369216402</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.05</v>
       </c>
       <c r="B30">
-        <v>0.81529411764705795</v>
+        <v>0.81</v>
       </c>
       <c r="C30">
-        <v>0.84</v>
-      </c>
-      <c r="D30">
-        <v>0.81529411764705795</v>
-      </c>
-      <c r="E30">
-        <v>0.84</v>
-      </c>
-      <c r="G30">
-        <v>0.05</v>
-      </c>
-      <c r="H30">
-        <v>0.82764705882352896</v>
-      </c>
-      <c r="I30">
-        <v>0.85</v>
+        <v>0.84331766509984296</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.1</v>
       </c>
       <c r="B31">
-        <v>0.81411764705882295</v>
+        <v>0.81352941176470495</v>
       </c>
       <c r="C31">
-        <v>0.83</v>
-      </c>
-      <c r="G31">
-        <v>0.1</v>
-      </c>
-      <c r="H31">
-        <v>0.83176470588235296</v>
-      </c>
-      <c r="I31">
-        <v>0.85666666666666602</v>
+        <v>0.83332592559669305</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.5</v>
       </c>
       <c r="B32">
-        <v>0.80705882352941105</v>
+        <v>0.80235294117647005</v>
       </c>
       <c r="C32">
-        <v>0.836666666666666</v>
-      </c>
-      <c r="G32">
-        <v>0.5</v>
-      </c>
-      <c r="H32">
-        <v>0.82</v>
-      </c>
-      <c r="I32">
-        <v>0.85666666666666602</v>
+        <v>0.84333159257324997</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="G35" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>500</v>
       </c>
       <c r="B36">
-        <v>0.82705882352941096</v>
+        <v>0.79176470588235204</v>
       </c>
       <c r="C36">
-        <v>0.83</v>
-      </c>
-      <c r="G36">
-        <v>500</v>
-      </c>
-      <c r="H36">
-        <v>0.83470588235294096</v>
-      </c>
-      <c r="I36">
-        <v>0.85666666666666602</v>
+        <v>0.81632175974886101</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1000</v>
       </c>
       <c r="B37">
-        <v>0.84529411764705797</v>
+        <v>0.81882352941176395</v>
       </c>
       <c r="C37">
-        <v>0.86333333333333295</v>
-      </c>
-      <c r="G37">
-        <v>1000</v>
-      </c>
-      <c r="H37">
-        <v>0.86</v>
-      </c>
-      <c r="I37">
-        <v>0.87333333333333296</v>
+        <v>0.86992918366666305</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1500</v>
       </c>
       <c r="B38">
-        <v>0.85588235294117598</v>
+        <v>0.82764705882352896</v>
       </c>
       <c r="C38">
-        <v>0.86</v>
-      </c>
-      <c r="G38">
-        <v>1500</v>
-      </c>
-      <c r="H38">
-        <v>0.86</v>
-      </c>
-      <c r="I38">
-        <v>0.87333333333333296</v>
+        <v>0.87997866287339899</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2000</v>
       </c>
       <c r="B39">
-        <v>0.85235294117646998</v>
+        <v>0.83235294117646996</v>
       </c>
       <c r="C39">
-        <v>0.87333333333333296</v>
-      </c>
-      <c r="G39">
-        <v>2000</v>
-      </c>
-      <c r="H39">
-        <v>0.86</v>
-      </c>
-      <c r="I39">
-        <v>0.86</v>
+        <v>0.85994397759103602</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2500</v>
       </c>
       <c r="B40">
-        <v>0.85</v>
+        <v>0.82823529411764696</v>
       </c>
       <c r="C40">
-        <v>0.87</v>
-      </c>
-      <c r="G40">
-        <v>2500</v>
-      </c>
-      <c r="H40">
-        <v>0.86764705882352899</v>
-      </c>
-      <c r="I40">
-        <v>0.88333333333333297</v>
+        <v>0.86992918366666305</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3000</v>
       </c>
       <c r="B41">
-        <v>0.85352941176470498</v>
+        <v>0.82705882352941096</v>
       </c>
       <c r="C41">
-        <v>0.87333333333333296</v>
-      </c>
-      <c r="G41">
-        <v>3000</v>
-      </c>
-      <c r="H41">
-        <v>0.871176470588235</v>
-      </c>
-      <c r="I41">
-        <v>0.9</v>
+        <v>0.876555566676675</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D42">
-        <v>0.81352941176470495</v>
-      </c>
-      <c r="E42">
-        <v>0.85333333333333306</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
-      <c r="D43">
-        <v>0.82882352941176396</v>
-      </c>
-      <c r="E43">
-        <v>0.84</v>
-      </c>
-      <c r="G43" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1E-3</v>
       </c>
       <c r="B44">
-        <v>0.85294117647058798</v>
+        <v>0.80764705882352905</v>
       </c>
       <c r="C44">
-        <v>0.85</v>
-      </c>
-      <c r="D44">
-        <v>0.84588235294117597</v>
-      </c>
-      <c r="E44">
-        <v>0.85333333333333306</v>
-      </c>
-      <c r="G44">
-        <v>1E-3</v>
-      </c>
-      <c r="H44">
-        <v>0.83294117647058796</v>
-      </c>
-      <c r="I44">
-        <v>0.88</v>
+        <v>0.85322896281800298</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B45">
-        <v>0.84117647058823497</v>
+        <v>0.81705882352941095</v>
       </c>
       <c r="C45">
-        <v>0.85333333333333306</v>
-      </c>
-      <c r="D45">
-        <v>0.84058823529411697</v>
-      </c>
-      <c r="E45">
-        <v>0.86</v>
-      </c>
-      <c r="G45">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H45">
-        <v>0.85823529411764699</v>
-      </c>
-      <c r="I45">
-        <v>0.87666666666666604</v>
+        <v>0.88994007848717605</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0.01</v>
       </c>
       <c r="B46">
-        <v>0.85529411764705798</v>
+        <v>0.82176470588235295</v>
       </c>
       <c r="C46">
-        <v>0.87666666666666604</v>
-      </c>
-      <c r="D46">
-        <v>0.85058823529411698</v>
-      </c>
-      <c r="E46">
-        <v>0.86666666666666603</v>
-      </c>
-      <c r="G46">
-        <v>0.01</v>
-      </c>
-      <c r="H46">
-        <v>0.85411764705882298</v>
-      </c>
-      <c r="I46">
-        <v>0.89333333333333298</v>
+        <v>0.86661331199146296</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0.05</v>
       </c>
       <c r="B47">
-        <v>0.85</v>
+        <v>0.83235294117646996</v>
       </c>
       <c r="C47">
-        <v>0.85666666666666602</v>
-      </c>
-      <c r="D47">
-        <v>0.84705882352941098</v>
-      </c>
-      <c r="E47">
-        <v>0.87333333333333296</v>
-      </c>
-      <c r="G47">
-        <v>0.05</v>
-      </c>
-      <c r="H47">
-        <v>0.85647058823529398</v>
-      </c>
-      <c r="I47">
-        <v>0.88</v>
+        <v>0.85977564102563997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0.1</v>
       </c>
       <c r="B48">
-        <v>0.86352941176470499</v>
+        <v>0.83235294117646996</v>
       </c>
       <c r="C48">
-        <v>0.88</v>
-      </c>
-      <c r="G48">
-        <v>0.1</v>
-      </c>
-      <c r="H48">
-        <v>0.87</v>
-      </c>
-      <c r="I48">
-        <v>0.89666666666666595</v>
+        <v>0.86967418546365904</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0.5</v>
       </c>
       <c r="B49">
-        <v>0.84470588235294097</v>
+        <v>0.83176470588235296</v>
       </c>
       <c r="C49">
-        <v>0.88</v>
-      </c>
-      <c r="G49">
-        <v>0.5</v>
-      </c>
-      <c r="H49">
-        <v>0.86352941176470499</v>
-      </c>
-      <c r="I49">
-        <v>0.92333333333333301</v>
+        <v>0.88326978021367097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>